<commit_message>
a simple ui touch
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\remi-polban\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -106,7 +106,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -480,11 +480,20 @@
         <color indexed="64"/>
       </diagonal>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -640,6 +649,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7090,7 +7105,7 @@
   <dimension ref="A1:DP51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CO6" sqref="CO6"/>
+      <selection activeCell="CB12" sqref="CB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10761,57 +10776,75 @@
       <c r="G31" s="27"/>
       <c r="H31" s="31"/>
       <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
+      <c r="J31" s="65">
+        <v>1</v>
+      </c>
+      <c r="K31" s="65"/>
       <c r="L31" s="31"/>
       <c r="M31" s="31"/>
       <c r="N31" s="21"/>
       <c r="O31" s="31"/>
       <c r="P31" s="31"/>
-      <c r="Q31" s="31"/>
-      <c r="R31" s="31"/>
+      <c r="Q31" s="65">
+        <v>2</v>
+      </c>
+      <c r="R31" s="65"/>
       <c r="S31" s="31"/>
       <c r="T31" s="31"/>
       <c r="U31" s="21"/>
       <c r="V31" s="31"/>
       <c r="W31" s="31"/>
-      <c r="X31" s="31"/>
-      <c r="Y31" s="31"/>
-      <c r="Z31" s="31"/>
+      <c r="X31" s="65">
+        <v>3</v>
+      </c>
+      <c r="Y31" s="65"/>
+      <c r="Z31" s="31">
+        <v>4</v>
+      </c>
       <c r="AA31" s="31"/>
       <c r="AB31" s="21"/>
       <c r="AC31" s="31"/>
       <c r="AD31" s="31"/>
-      <c r="AE31" s="31"/>
-      <c r="AF31" s="31"/>
+      <c r="AE31" s="65">
+        <v>4</v>
+      </c>
+      <c r="AF31" s="65"/>
       <c r="AG31" s="31"/>
       <c r="AH31" s="31"/>
       <c r="AI31" s="21"/>
       <c r="AJ31" s="31"/>
       <c r="AK31" s="31"/>
-      <c r="AL31" s="31"/>
-      <c r="AM31" s="31"/>
+      <c r="AL31" s="65">
+        <v>5</v>
+      </c>
+      <c r="AM31" s="65"/>
       <c r="AN31" s="31"/>
       <c r="AO31" s="31"/>
       <c r="AP31" s="21"/>
       <c r="AQ31" s="31"/>
       <c r="AR31" s="31"/>
-      <c r="AS31" s="31"/>
-      <c r="AT31" s="31"/>
+      <c r="AS31" s="65">
+        <v>6</v>
+      </c>
+      <c r="AT31" s="65"/>
       <c r="AU31" s="31"/>
       <c r="AV31" s="31"/>
       <c r="AW31" s="21"/>
       <c r="AX31" s="31"/>
       <c r="AY31" s="31"/>
-      <c r="AZ31" s="31"/>
-      <c r="BA31" s="31"/>
+      <c r="AZ31" s="65">
+        <v>7</v>
+      </c>
+      <c r="BA31" s="65"/>
       <c r="BB31" s="31"/>
       <c r="BC31" s="31"/>
       <c r="BD31" s="21"/>
       <c r="BE31" s="31"/>
       <c r="BF31" s="31"/>
-      <c r="BG31" s="31"/>
-      <c r="BH31" s="31"/>
+      <c r="BG31" s="65">
+        <v>8</v>
+      </c>
+      <c r="BH31" s="65"/>
       <c r="BI31" s="31"/>
       <c r="BJ31" s="31"/>
       <c r="BK31" s="27"/>
@@ -10883,57 +10916,57 @@
       <c r="G32" s="27"/>
       <c r="H32" s="31"/>
       <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
       <c r="L32" s="31"/>
       <c r="M32" s="31"/>
       <c r="N32" s="21"/>
       <c r="O32" s="31"/>
       <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="31"/>
+      <c r="Q32" s="65"/>
+      <c r="R32" s="65"/>
       <c r="S32" s="31"/>
       <c r="T32" s="31"/>
       <c r="U32" s="21"/>
       <c r="V32" s="31"/>
       <c r="W32" s="31"/>
-      <c r="X32" s="31"/>
-      <c r="Y32" s="31"/>
+      <c r="X32" s="65"/>
+      <c r="Y32" s="65"/>
       <c r="Z32" s="31"/>
       <c r="AA32" s="31"/>
       <c r="AB32" s="21"/>
       <c r="AC32" s="31"/>
       <c r="AD32" s="31"/>
-      <c r="AE32" s="31"/>
-      <c r="AF32" s="31"/>
+      <c r="AE32" s="65"/>
+      <c r="AF32" s="65"/>
       <c r="AG32" s="31"/>
       <c r="AH32" s="31"/>
       <c r="AI32" s="21"/>
       <c r="AJ32" s="31"/>
       <c r="AK32" s="31"/>
-      <c r="AL32" s="31"/>
-      <c r="AM32" s="31"/>
+      <c r="AL32" s="65"/>
+      <c r="AM32" s="65"/>
       <c r="AN32" s="31"/>
       <c r="AO32" s="31"/>
       <c r="AP32" s="21"/>
       <c r="AQ32" s="31"/>
       <c r="AR32" s="31"/>
-      <c r="AS32" s="31"/>
-      <c r="AT32" s="31"/>
+      <c r="AS32" s="65"/>
+      <c r="AT32" s="65"/>
       <c r="AU32" s="31"/>
       <c r="AV32" s="31"/>
       <c r="AW32" s="21"/>
       <c r="AX32" s="31"/>
       <c r="AY32" s="31"/>
-      <c r="AZ32" s="31"/>
-      <c r="BA32" s="31"/>
+      <c r="AZ32" s="65"/>
+      <c r="BA32" s="65"/>
       <c r="BB32" s="31"/>
       <c r="BC32" s="31"/>
       <c r="BD32" s="21"/>
       <c r="BE32" s="31"/>
       <c r="BF32" s="31"/>
-      <c r="BG32" s="31"/>
-      <c r="BH32" s="31"/>
+      <c r="BG32" s="65"/>
+      <c r="BH32" s="65"/>
       <c r="BI32" s="31"/>
       <c r="BJ32" s="31"/>
       <c r="BK32" s="27"/>
@@ -11005,57 +11038,57 @@
       <c r="G33" s="27"/>
       <c r="H33" s="31"/>
       <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="65"/>
       <c r="L33" s="31"/>
       <c r="M33" s="31"/>
       <c r="N33" s="21"/>
       <c r="O33" s="31"/>
       <c r="P33" s="31"/>
-      <c r="Q33" s="31"/>
-      <c r="R33" s="31"/>
+      <c r="Q33" s="65"/>
+      <c r="R33" s="65"/>
       <c r="S33" s="31"/>
       <c r="T33" s="31"/>
       <c r="U33" s="21"/>
       <c r="V33" s="31"/>
       <c r="W33" s="31"/>
-      <c r="X33" s="31"/>
-      <c r="Y33" s="31"/>
+      <c r="X33" s="65"/>
+      <c r="Y33" s="65"/>
       <c r="Z33" s="31"/>
       <c r="AA33" s="31"/>
       <c r="AB33" s="21"/>
       <c r="AC33" s="31"/>
       <c r="AD33" s="31"/>
-      <c r="AE33" s="31"/>
-      <c r="AF33" s="31"/>
+      <c r="AE33" s="65"/>
+      <c r="AF33" s="65"/>
       <c r="AG33" s="31"/>
       <c r="AH33" s="31"/>
       <c r="AI33" s="21"/>
       <c r="AJ33" s="31"/>
       <c r="AK33" s="31"/>
-      <c r="AL33" s="31"/>
-      <c r="AM33" s="31"/>
+      <c r="AL33" s="65"/>
+      <c r="AM33" s="65"/>
       <c r="AN33" s="31"/>
       <c r="AO33" s="31"/>
       <c r="AP33" s="21"/>
       <c r="AQ33" s="31"/>
       <c r="AR33" s="31"/>
-      <c r="AS33" s="31"/>
-      <c r="AT33" s="31"/>
+      <c r="AS33" s="65"/>
+      <c r="AT33" s="65"/>
       <c r="AU33" s="31"/>
       <c r="AV33" s="31"/>
       <c r="AW33" s="21"/>
       <c r="AX33" s="31"/>
       <c r="AY33" s="31"/>
-      <c r="AZ33" s="31"/>
-      <c r="BA33" s="31"/>
+      <c r="AZ33" s="65"/>
+      <c r="BA33" s="65"/>
       <c r="BB33" s="31"/>
       <c r="BC33" s="31"/>
       <c r="BD33" s="21"/>
       <c r="BE33" s="31"/>
       <c r="BF33" s="31"/>
-      <c r="BG33" s="31"/>
-      <c r="BH33" s="31"/>
+      <c r="BG33" s="65"/>
+      <c r="BH33" s="65"/>
       <c r="BI33" s="31"/>
       <c r="BJ33" s="31"/>
       <c r="BK33" s="27"/>
@@ -11126,59 +11159,75 @@
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
       <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
+      <c r="I34" s="66">
+        <v>9</v>
+      </c>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
       <c r="M34" s="31"/>
       <c r="N34" s="21"/>
       <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
-      <c r="Q34" s="31"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="31"/>
+      <c r="P34" s="66">
+        <v>16</v>
+      </c>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="66"/>
+      <c r="S34" s="66"/>
       <c r="T34" s="31"/>
       <c r="U34" s="21"/>
       <c r="V34" s="31"/>
-      <c r="W34" s="31"/>
-      <c r="X34" s="31"/>
-      <c r="Y34" s="31"/>
-      <c r="Z34" s="31"/>
+      <c r="W34" s="66">
+        <v>23</v>
+      </c>
+      <c r="X34" s="66"/>
+      <c r="Y34" s="66"/>
+      <c r="Z34" s="66"/>
       <c r="AA34" s="31"/>
       <c r="AB34" s="21"/>
       <c r="AC34" s="31"/>
-      <c r="AD34" s="31"/>
-      <c r="AE34" s="31"/>
-      <c r="AF34" s="31"/>
-      <c r="AG34" s="31"/>
+      <c r="AD34" s="66">
+        <v>30</v>
+      </c>
+      <c r="AE34" s="66"/>
+      <c r="AF34" s="66"/>
+      <c r="AG34" s="66"/>
       <c r="AH34" s="31"/>
       <c r="AI34" s="21"/>
       <c r="AJ34" s="31"/>
-      <c r="AK34" s="31"/>
-      <c r="AL34" s="31"/>
-      <c r="AM34" s="31"/>
-      <c r="AN34" s="31"/>
+      <c r="AK34" s="66">
+        <v>37</v>
+      </c>
+      <c r="AL34" s="66"/>
+      <c r="AM34" s="66"/>
+      <c r="AN34" s="66"/>
       <c r="AO34" s="31"/>
       <c r="AP34" s="21"/>
       <c r="AQ34" s="31"/>
-      <c r="AR34" s="31"/>
-      <c r="AS34" s="31"/>
-      <c r="AT34" s="31"/>
-      <c r="AU34" s="31"/>
+      <c r="AR34" s="66">
+        <v>44</v>
+      </c>
+      <c r="AS34" s="66"/>
+      <c r="AT34" s="66"/>
+      <c r="AU34" s="66"/>
       <c r="AV34" s="31"/>
       <c r="AW34" s="21"/>
       <c r="AX34" s="31"/>
-      <c r="AY34" s="31"/>
-      <c r="AZ34" s="31"/>
-      <c r="BA34" s="31"/>
-      <c r="BB34" s="31"/>
+      <c r="AY34" s="66">
+        <v>51</v>
+      </c>
+      <c r="AZ34" s="66"/>
+      <c r="BA34" s="66"/>
+      <c r="BB34" s="66"/>
       <c r="BC34" s="31"/>
       <c r="BD34" s="21"/>
       <c r="BE34" s="31"/>
-      <c r="BF34" s="31"/>
-      <c r="BG34" s="31"/>
-      <c r="BH34" s="31"/>
-      <c r="BI34" s="31"/>
+      <c r="BF34" s="66">
+        <v>58</v>
+      </c>
+      <c r="BG34" s="66"/>
+      <c r="BH34" s="66"/>
+      <c r="BI34" s="66"/>
       <c r="BJ34" s="31"/>
       <c r="BK34" s="27"/>
       <c r="BL34" s="27"/>
@@ -13284,6 +13333,24 @@
       <c r="DP51" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="AY34:BB34"/>
+    <mergeCell ref="BF34:BI34"/>
+    <mergeCell ref="P34:S34"/>
+    <mergeCell ref="I34:L34"/>
+    <mergeCell ref="W34:Z34"/>
+    <mergeCell ref="AD34:AG34"/>
+    <mergeCell ref="AK34:AN34"/>
+    <mergeCell ref="AR34:AU34"/>
+    <mergeCell ref="AZ31:BA33"/>
+    <mergeCell ref="BG31:BH33"/>
+    <mergeCell ref="J31:K33"/>
+    <mergeCell ref="Q31:R33"/>
+    <mergeCell ref="X31:Y33"/>
+    <mergeCell ref="AE31:AF33"/>
+    <mergeCell ref="AL31:AM33"/>
+    <mergeCell ref="AS31:AT33"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>